<commit_message>
Set substringo of rich text to Garamond font, instead of Broadway. Broadway probably isn't installed on the AppVeyor server. Garamond is a much more common pre-installed font.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -31,7 +31,7 @@
         <x:vertAlign val="baseline"/>
         <x:sz val="11"/>
         <x:color rgb="FFFF0000"/>
-        <x:rFont val="Broadway"/>
+        <x:rFont val="Garamond"/>
         <x:family val="2"/>
       </x:rPr>
       <x:t>show</x:t>
@@ -475,7 +475,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="22.520625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="21.160625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="14.060625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>

<commit_message>
Disable different font to see if it affects the AppVeyor build.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -31,7 +31,7 @@
         <x:vertAlign val="baseline"/>
         <x:sz val="11"/>
         <x:color rgb="FFFF0000"/>
-        <x:rFont val="Garamond"/>
+        <x:rFont val="Calibri"/>
         <x:family val="2"/>
       </x:rPr>
       <x:t>show</x:t>
@@ -475,7 +475,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="21.160625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="21.380625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="14.060625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>

<commit_message>
Use Courier font for rich text. Hopefully this one is installed on AppVeyor.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -31,7 +31,7 @@
         <x:vertAlign val="baseline"/>
         <x:sz val="11"/>
         <x:color rgb="FFFF0000"/>
-        <x:rFont val="Calibri"/>
+        <x:rFont val="Courier"/>
         <x:family val="2"/>
       </x:rPr>
       <x:t>show</x:t>
@@ -475,7 +475,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="21.380625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="21.750625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="14.060625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>

<commit_message>
When setting cell value to RichText, don't use SetEnumerable.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/UsingRichText.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
     <x:r>
       <x:rPr>
@@ -105,6 +105,74 @@
   </x:si>
   <x:si>
     <x:t>" BIG " is Bold.</x:t>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF008000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Some</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:b/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF0000FF"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t xml:space="preserve"> rich text </x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:i/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>with a gray background</x:t>
+    </x:r>
+  </x:si>
+  <x:si>
+    <x:r>
+      <x:rPr>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF008000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>Some</x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:b/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF0000FF"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t xml:space="preserve"> rich text </x:t>
+    </x:r>
+    <x:r>
+      <x:rPr>
+        <x:i/>
+        <x:vertAlign val="baseline"/>
+        <x:sz val="11"/>
+        <x:color rgb="FF000000"/>
+        <x:rFont val="Calibri"/>
+        <x:family val="2"/>
+      </x:rPr>
+      <x:t>with a gray background</x:t>
+    </x:r>
   </x:si>
 </x:sst>
 </file>
@@ -130,13 +198,19 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF808080"/>
+        <x:bgColor rgb="FF808080"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
   <x:borders count="1">
     <x:border diagonalUp="0" diagonalDown="0">
@@ -157,20 +231,27 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -469,14 +550,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B3"/>
+  <x:dimension ref="A1:B5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="21.750625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="14.060625" style="0" customWidth="1"/>
+    <x:col min="1" max="2" width="34.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2">
@@ -492,6 +572,14 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>